<commit_message>
Additional edits to handle sheet specific needs
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C812DED-2734-4531-A001-AB0446933E91}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="113">
   <si>
     <t>from</t>
   </si>
@@ -102,9 +102,6 @@
     <t>dose_vehicle</t>
   </si>
   <si>
-    <t>dose_volume</t>
-  </si>
-  <si>
     <t>fasting_period</t>
   </si>
   <si>
@@ -162,12 +159,6 @@
     <t>height_units</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>weight_units</t>
-  </si>
-  <si>
     <t>analyte_name</t>
   </si>
   <si>
@@ -255,21 +246,6 @@
     <t>conc_upper_bound</t>
   </si>
   <si>
-    <t>test_substance_name_original</t>
-  </si>
-  <si>
-    <t>dose_level_original</t>
-  </si>
-  <si>
-    <t>dose_level_original_units</t>
-  </si>
-  <si>
-    <t>administration_route_original</t>
-  </si>
-  <si>
-    <t>analyte_name_original</t>
-  </si>
-  <si>
     <t>conc_units_original</t>
   </si>
   <si>
@@ -279,12 +255,6 @@
     <t>log_units</t>
   </si>
   <si>
-    <t>time_units_original</t>
-  </si>
-  <si>
-    <t>time_original</t>
-  </si>
-  <si>
     <t>conc_original</t>
   </si>
   <si>
@@ -321,12 +291,6 @@
     <t>test_substance_name_secondary_original</t>
   </si>
   <si>
-    <t>test_substance_casrn_original</t>
-  </si>
-  <si>
-    <t>dose_volume_units</t>
-  </si>
-  <si>
     <t>extracted</t>
   </si>
   <si>
@@ -352,6 +316,66 @@
   </si>
   <si>
     <t>qc_flags</t>
+  </si>
+  <si>
+    <t>Animal ID</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Test Article</t>
+  </si>
+  <si>
+    <t>CASRN</t>
+  </si>
+  <si>
+    <t>Dose</t>
+  </si>
+  <si>
+    <t>Dose Unit</t>
+  </si>
+  <si>
+    <t>Volume Per Admin (mL/kg)</t>
+  </si>
+  <si>
+    <t>Dose Frequency (Per Study)</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Initial Body Weight (g)</t>
+  </si>
+  <si>
+    <t>Target Point</t>
+  </si>
+  <si>
+    <t>Target Point Unit</t>
+  </si>
+  <si>
+    <t>Analyte</t>
+  </si>
+  <si>
+    <t>Brain Concentration (ng/g)</t>
+  </si>
+  <si>
+    <t>Brain Concentration Specification</t>
+  </si>
+  <si>
+    <t>Plasma Concentration (ng/mL)</t>
+  </si>
+  <si>
+    <t>Plasma Concentration Specification</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
   </si>
 </sst>
 </file>
@@ -367,12 +391,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -387,8 +417,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,16 +735,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100:C102"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
     <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -729,7 +761,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -740,29 +772,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -773,7 +805,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -784,7 +816,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -795,7 +827,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -806,7 +838,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -817,7 +849,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -828,7 +860,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -839,7 +871,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -850,62 +882,62 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -916,21 +948,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -938,10 +970,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -949,10 +981,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" t="s">
-        <v>94</v>
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -960,10 +992,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -971,10 +1003,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -982,10 +1014,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -993,29 +1025,29 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -1026,10 +1058,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -1037,40 +1069,40 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>21</v>
+        <v>77</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>95</v>
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
         <v>22</v>
@@ -1081,29 +1113,29 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>24</v>
@@ -1114,7 +1146,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -1125,7 +1157,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
         <v>26</v>
@@ -1136,7 +1168,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>27</v>
@@ -1147,7 +1179,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
@@ -1158,7 +1190,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>29</v>
@@ -1169,7 +1201,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
@@ -1180,7 +1212,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -1191,65 +1223,65 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" t="s">
-        <v>33</v>
+        <v>78</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
@@ -1257,10 +1289,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
+        <v>78</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
@@ -1268,578 +1300,699 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
         <v>36</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
         <v>37</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
         <v>38</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
         <v>39</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
+        <v>78</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57" t="s">
-        <v>41</v>
-      </c>
-      <c r="C57" t="s">
-        <v>41</v>
+        <v>78</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" t="s">
-        <v>42</v>
+        <v>90</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" t="s">
-        <v>9</v>
+        <v>91</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" t="s">
-        <v>104</v>
+        <v>79</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>89</v>
-      </c>
-      <c r="B73" t="s">
-        <v>52</v>
+        <v>79</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C73" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="C76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C87" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>103</v>
+        <v>79</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C90" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" t="s">
-        <v>104</v>
+        <v>79</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" t="s">
-        <v>11</v>
+        <v>79</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C93" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>90</v>
-      </c>
-      <c r="B94" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>90</v>
-      </c>
-      <c r="B96" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C96" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>90</v>
-      </c>
-      <c r="B97" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>90</v>
-      </c>
-      <c r="B100" t="s">
-        <v>102</v>
+        <v>80</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C100" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>80</v>
+      </c>
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" t="s">
+        <v>74</v>
+      </c>
+      <c r="C104" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>80</v>
+      </c>
+      <c r="B106" t="s">
         <v>90</v>
       </c>
-      <c r="B102" t="s">
-        <v>104</v>
-      </c>
-      <c r="C102" t="s">
-        <v>104</v>
+      <c r="C106" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" t="s">
+        <v>91</v>
+      </c>
+      <c r="C107" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>80</v>
+      </c>
+      <c r="B108" t="s">
+        <v>92</v>
+      </c>
+      <c r="C108" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>80</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>80</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C113" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C99" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C104" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Increased dynamic capabilities, added conc_time_values curator_comment, added foreign keys
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C812DED-2734-4531-A001-AB0446933E91}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A97AAF7-E247-440A-AC45-AB394A58AF7B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="109">
   <si>
     <t>from</t>
   </si>
@@ -361,18 +361,6 @@
   </si>
   <si>
     <t>Analyte</t>
-  </si>
-  <si>
-    <t>Brain Concentration (ng/g)</t>
-  </si>
-  <si>
-    <t>Brain Concentration Specification</t>
-  </si>
-  <si>
-    <t>Plasma Concentration (ng/mL)</t>
-  </si>
-  <si>
-    <t>Plasma Concentration Specification</t>
   </si>
   <si>
     <t>sheet_name</t>
@@ -735,20 +723,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -759,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -770,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -781,7 +769,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -792,7 +780,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -803,7 +791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -814,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -825,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -836,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -847,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -858,7 +846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -869,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -880,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -891,7 +879,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -902,7 +890,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -913,7 +901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -924,7 +912,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -935,7 +923,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -946,7 +934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -957,7 +945,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -968,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -979,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -990,7 +978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1001,7 +989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1012,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1023,7 +1011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1034,7 +1022,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1045,7 +1033,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -1056,7 +1044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -1067,7 +1055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1078,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1089,7 +1077,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -1100,7 +1088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1111,7 +1099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -1122,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -1133,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -1144,7 +1132,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1155,7 +1143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -1166,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1177,7 +1165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1188,7 +1176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1199,7 +1187,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -1210,7 +1198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1221,7 +1209,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1232,7 +1220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1243,7 +1231,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1254,7 +1242,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1265,7 +1253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -1276,7 +1264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -1287,7 +1275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1298,7 +1286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -1309,7 +1297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -1320,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -1331,7 +1319,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -1342,7 +1330,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -1353,7 +1341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -1364,7 +1352,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -1375,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -1386,7 +1374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -1397,7 +1385,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -1408,7 +1396,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -1419,7 +1407,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1430,7 +1418,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -1441,7 +1429,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -1452,7 +1440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -1463,7 +1451,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1474,7 +1462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1485,7 +1473,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -1496,7 +1484,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1507,7 +1495,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -1518,7 +1506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -1529,7 +1517,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -1540,7 +1528,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -1551,7 +1539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -1562,7 +1550,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -1573,7 +1561,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -1584,7 +1572,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -1595,7 +1583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -1606,7 +1594,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -1617,7 +1605,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1628,7 +1616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1639,7 +1627,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -1650,7 +1638,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -1661,7 +1649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>79</v>
       </c>
@@ -1672,7 +1660,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -1683,7 +1671,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -1694,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>79</v>
       </c>
@@ -1705,7 +1693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>79</v>
       </c>
@@ -1716,7 +1704,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>79</v>
       </c>
@@ -1727,18 +1715,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>79</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>79</v>
       </c>
@@ -1749,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -1760,239 +1748,184 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>79</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" s="1" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C95" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>79</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>79</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>105</v>
+        <v>80</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>80</v>
       </c>
-      <c r="B99" t="s">
-        <v>63</v>
+      <c r="B99" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C99" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>80</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>105</v>
+      <c r="B100" t="s">
+        <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>80</v>
       </c>
       <c r="B101" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C101" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>80</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C102" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>80</v>
       </c>
       <c r="B103" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>80</v>
       </c>
       <c r="B104" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>80</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C105" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C106" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>80</v>
       </c>
       <c r="B107" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C107" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>80</v>
       </c>
-      <c r="B108" t="s">
-        <v>92</v>
+      <c r="B108" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C108" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C109" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>80</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>80</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>80</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C112" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>80</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C113" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C104" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C103" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handling multiple weight fields and de-duping subjects
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A97AAF7-E247-440A-AC45-AB394A58AF7B}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E2DCCE-8BEA-42B6-ADE7-72E190B14710}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
@@ -351,9 +351,6 @@
     <t>Route</t>
   </si>
   <si>
-    <t>Initial Body Weight (g)</t>
-  </si>
-  <si>
     <t>Target Point</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Dose Frequency (per Study)</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
         <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -1059,33 +1059,33 @@
       <c r="A30" t="s">
         <v>77</v>
       </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>20</v>
+      <c r="B30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>101</v>
+      <c r="B31" t="s">
+        <v>20</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
-      <c r="B32" t="s">
-        <v>21</v>
+      <c r="B32" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,10 +1093,10 @@
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1104,10 +1104,10 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,10 +1115,10 @@
         <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,10 +1126,10 @@
         <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,10 +1137,10 @@
         <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,10 +1148,10 @@
         <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1159,10 @@
         <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,10 +1170,10 @@
         <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,10 +1192,10 @@
         <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,10 +1203,10 @@
         <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,10 +1214,10 @@
         <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1225,10 @@
         <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,32 +1236,32 @@
         <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>94</v>
+      <c r="B48" t="s">
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,21 +1280,21 @@
         <v>78</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>78</v>
       </c>
-      <c r="B51" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>35</v>
+      <c r="B51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,10 +1302,10 @@
         <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,10 +1313,10 @@
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,10 +1324,10 @@
         <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,21 +1335,21 @@
         <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>104</v>
+      <c r="B56" t="s">
+        <v>39</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>79</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
         <v>40</v>
@@ -1533,7 +1533,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C73" t="s">
         <v>50</v>
@@ -1720,10 +1720,10 @@
         <v>79</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1786,7 +1786,7 @@
         <v>79</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96" t="s">
         <v>64</v>
@@ -1819,7 +1819,7 @@
         <v>80</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C99" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Various cases handled from additional test file
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E2DCCE-8BEA-42B6-ADE7-72E190B14710}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A39B9D0C-813C-4F14-8468-82C543E7DD35}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="111">
   <si>
     <t>from</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>Dose Frequency (per Study)</t>
+  </si>
+  <si>
+    <t>Dose Frequency (per study)</t>
+  </si>
+  <si>
+    <t>Dose Frequency (Per study)</t>
   </si>
 </sst>
 </file>
@@ -723,20 +729,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -747,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -758,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -769,7 +775,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -780,7 +786,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -791,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -802,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -813,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -824,7 +830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -835,7 +841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -846,7 +852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -857,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -868,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -879,7 +885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -890,7 +896,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -901,7 +907,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -912,7 +918,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -923,7 +929,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -934,7 +940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -945,7 +951,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -956,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -967,7 +973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -978,7 +984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -989,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1066,866 +1072,899 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
         <v>22</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
         <v>23</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
         <v>24</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
         <v>25</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
         <v>26</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
         <v>27</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
         <v>29</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" t="s">
         <v>30</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
         <v>31</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
         <v>90</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
         <v>91</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" t="s">
         <v>92</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>95</v>
+      <c r="B50" t="s">
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>78</v>
       </c>
-      <c r="B52" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>78</v>
       </c>
-      <c r="B53" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>93</v>
+      <c r="B57" t="s">
+        <v>38</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>78</v>
       </c>
-      <c r="B59" t="s">
-        <v>91</v>
+      <c r="B59" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>78</v>
       </c>
       <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" t="s">
         <v>92</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>79</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>79</v>
-      </c>
-      <c r="B62" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" t="s">
         <v>41</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>79</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" t="s">
         <v>42</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
         <v>43</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>79</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" t="s">
         <v>44</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" t="s">
         <v>45</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>79</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" t="s">
         <v>46</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>79</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" t="s">
         <v>47</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" t="s">
         <v>48</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
         <v>49</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>79</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="s">
         <v>87</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="1" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
         <v>69</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
         <v>71</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" t="s">
         <v>53</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
         <v>54</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>79</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>55</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
         <v>56</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
         <v>57</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" t="s">
         <v>58</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>79</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
         <v>59</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" t="s">
         <v>60</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>79</v>
-      </c>
-      <c r="B84" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" t="s">
         <v>61</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" t="s">
         <v>70</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>79</v>
-      </c>
-      <c r="B86" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" t="s">
         <v>9</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>79</v>
-      </c>
-      <c r="B87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" t="s">
         <v>90</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C89" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>79</v>
-      </c>
-      <c r="B88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" t="s">
         <v>91</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" t="s">
         <v>92</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>79</v>
-      </c>
-      <c r="B90" s="1" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" s="1" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C93" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C94" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="1" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" s="1" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C96" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="1" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" s="1" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>80</v>
-      </c>
-      <c r="B97" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>80</v>
-      </c>
-      <c r="B98" t="s">
-        <v>63</v>
-      </c>
-      <c r="C98" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>80</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>80</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C101" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>80</v>
       </c>
-      <c r="B102" t="s">
-        <v>73</v>
+      <c r="B102" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>80</v>
       </c>
       <c r="B103" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>80</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C104" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>80</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C105" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C106" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>80</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>80</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
+        <v>90</v>
+      </c>
+      <c r="C108" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" t="s">
+        <v>91</v>
+      </c>
+      <c r="C109" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>80</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C111" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C103" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C106" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to NTP auto-extraction cases
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A39B9D0C-813C-4F14-8468-82C543E7DD35}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC97E800-4725-4EA9-97A5-0BB6328B7CAA}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="4908" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
   <si>
     <t>from</t>
   </si>
@@ -96,9 +96,6 @@
     <t>dose_duration</t>
   </si>
   <si>
-    <t>dose_frequency</t>
-  </si>
-  <si>
     <t>dose_vehicle</t>
   </si>
   <si>
@@ -342,12 +339,6 @@
     <t>Dose Unit</t>
   </si>
   <si>
-    <t>Volume Per Admin (mL/kg)</t>
-  </si>
-  <si>
-    <t>Dose Frequency (Per Study)</t>
-  </si>
-  <si>
     <t>Route</t>
   </si>
   <si>
@@ -361,15 +352,6 @@
   </si>
   <si>
     <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Dose Frequency (per Study)</t>
-  </si>
-  <si>
-    <t>Dose Frequency (per study)</t>
-  </si>
-  <si>
-    <t>Dose Frequency (Per study)</t>
   </si>
 </sst>
 </file>
@@ -729,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +737,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -766,29 +748,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -799,7 +781,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -810,7 +792,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -821,7 +803,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -832,7 +814,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -843,7 +825,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -854,7 +836,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -865,7 +847,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -876,62 +858,62 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -942,21 +924,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -964,10 +946,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -975,10 +957,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -986,10 +968,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -997,10 +979,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -1008,10 +990,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1019,29 +1001,29 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -1052,178 +1034,178 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>101</v>
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1231,18 +1213,18 @@
         <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>77</v>
       </c>
-      <c r="B46" t="s">
-        <v>31</v>
+      <c r="B46" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C46" t="s">
         <v>31</v>
@@ -1252,22 +1234,22 @@
       <c r="A47" t="s">
         <v>77</v>
       </c>
-      <c r="B47" t="s">
-        <v>90</v>
+      <c r="B47" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>77</v>
       </c>
-      <c r="B48" t="s">
-        <v>91</v>
+      <c r="B48" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1275,98 +1257,98 @@
         <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" t="s">
-        <v>92</v>
+        <v>34</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" t="s">
-        <v>32</v>
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" t="s">
-        <v>33</v>
+        <v>77</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" t="s">
-        <v>34</v>
+        <v>77</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" t="s">
-        <v>35</v>
+        <v>77</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>38</v>
+        <v>91</v>
+      </c>
+      <c r="C57" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1374,10 +1356,10 @@
         <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1385,10 +1367,10 @@
         <v>78</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>9</v>
+        <v>103</v>
+      </c>
+      <c r="C59" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1396,10 +1378,10 @@
         <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>90</v>
+        <v>40</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1407,10 +1389,10 @@
         <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>91</v>
+        <v>41</v>
+      </c>
+      <c r="C61" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1418,384 +1400,384 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>79</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>106</v>
+        <v>78</v>
+      </c>
+      <c r="B64" t="s">
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C65" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C67" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" t="s">
-        <v>46</v>
+        <v>78</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>105</v>
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C77" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C78" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C81" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C85" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C86" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>79</v>
-      </c>
-      <c r="B87" t="s">
-        <v>70</v>
+        <v>78</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="C87" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>79</v>
-      </c>
-      <c r="B88" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="C89" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>79</v>
-      </c>
-      <c r="B90" t="s">
-        <v>91</v>
+        <v>78</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C91" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>107</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C93" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>98</v>
+      <c r="B95" t="s">
+        <v>11</v>
       </c>
       <c r="C95" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>79</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>99</v>
+      <c r="B96" t="s">
+        <v>62</v>
       </c>
       <c r="C96" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -1803,18 +1785,18 @@
         <v>79</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>79</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>104</v>
+      <c r="B98" t="s">
+        <v>71</v>
       </c>
       <c r="C98" t="s">
         <v>64</v>
@@ -1824,143 +1806,88 @@
       <c r="A99" t="s">
         <v>79</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>96</v>
+      <c r="B99" t="s">
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B100" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B101" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C101" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>80</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>104</v>
+        <v>79</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C103" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C104" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B105" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C105" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>80</v>
-      </c>
-      <c r="B106" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C106" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>80</v>
-      </c>
-      <c r="B107" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>80</v>
-      </c>
-      <c r="B108" t="s">
-        <v>90</v>
-      </c>
-      <c r="C108" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" t="s">
-        <v>91</v>
-      </c>
-      <c r="C109" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>80</v>
-      </c>
-      <c r="B110" t="s">
-        <v>92</v>
-      </c>
-      <c r="C110" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>80</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C111" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handling of additional cases
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC97E800-4725-4EA9-97A5-0BB6328B7CAA}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB8A82BA-5D38-420D-A15A-FF30C99FC596}"/>
   <bookViews>
-    <workbookView xWindow="4908" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$107</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="105">
   <si>
     <t>from</t>
   </si>
@@ -711,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,10 +1730,10 @@
         <v>78</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1741,10 +1741,10 @@
         <v>78</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -1752,21 +1752,21 @@
         <v>78</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C94" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -1774,32 +1774,32 @@
         <v>79</v>
       </c>
       <c r="B96" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>79</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>101</v>
+      <c r="B97" t="s">
+        <v>62</v>
       </c>
       <c r="C97" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>79</v>
       </c>
-      <c r="B98" t="s">
-        <v>71</v>
+      <c r="B98" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -1807,10 +1807,10 @@
         <v>79</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C99" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -1818,10 +1818,10 @@
         <v>79</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1829,10 +1829,10 @@
         <v>79</v>
       </c>
       <c r="B101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -1840,10 +1840,10 @@
         <v>79</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -1851,10 +1851,10 @@
         <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -1862,10 +1862,10 @@
         <v>79</v>
       </c>
       <c r="B104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -1873,25 +1873,36 @@
         <v>79</v>
       </c>
       <c r="B105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>79</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C106" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C107" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reorganize NTP extraction, update dictionary.
</commit_message>
<xml_diff>
--- a/input/ntp_template_map.xlsx
+++ b/input/ntp_template_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB8A82BA-5D38-420D-A15A-FF30C99FC596}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4AFFB00-9E88-4ADB-87F8-3D279140B56E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="31455" yWindow="4185" windowWidth="21600" windowHeight="11235" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$109</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="106">
   <si>
     <t>from</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Actual Sample Time</t>
   </si>
 </sst>
 </file>
@@ -412,6 +415,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,20 +718,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -735,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -746,7 +753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -757,7 +764,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -768,7 +775,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -779,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -790,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -801,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -812,7 +819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -823,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -834,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -845,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -856,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -867,7 +874,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -878,7 +885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -889,7 +896,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -900,7 +907,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -911,7 +918,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -922,7 +929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -933,7 +940,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -944,7 +951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -955,7 +962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -966,7 +973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -977,7 +984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -988,7 +995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1021,7 +1028,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1032,7 +1039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1043,7 +1050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1120,7 +1127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1131,7 +1138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1153,7 +1160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1164,7 +1171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -1186,7 +1193,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -1208,7 +1215,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1230,7 +1237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1241,7 +1248,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -1252,7 +1259,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -1318,7 +1325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -1351,7 +1358,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -1362,7 +1369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -1373,7 +1380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -1395,7 +1402,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -1472,7 +1479,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -1505,7 +1512,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -1582,7 +1589,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1604,7 +1611,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -1615,7 +1622,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -1626,7 +1633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -1637,7 +1644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>78</v>
       </c>
@@ -1648,7 +1655,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>78</v>
       </c>
@@ -1659,7 +1666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>78</v>
       </c>
@@ -1670,7 +1677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>78</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>78</v>
       </c>
@@ -1692,7 +1699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>78</v>
       </c>
@@ -1703,7 +1710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>78</v>
       </c>
@@ -1714,7 +1721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -1725,7 +1732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>78</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>78</v>
       </c>
@@ -1747,7 +1754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>78</v>
       </c>
@@ -1758,151 +1765,173 @@
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>78</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C95" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>79</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>101</v>
+      <c r="B98" t="s">
+        <v>62</v>
       </c>
       <c r="C98" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>79</v>
       </c>
-      <c r="B99" t="s">
-        <v>71</v>
+      <c r="B99" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>79</v>
       </c>
-      <c r="B100" t="s">
-        <v>74</v>
+      <c r="B100" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C100" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>79</v>
       </c>
       <c r="B101" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C101" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>79</v>
       </c>
       <c r="B102" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>79</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C104" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>79</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>79</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C106" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>79</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
+        <v>90</v>
+      </c>
+      <c r="C107" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" t="s">
+        <v>91</v>
+      </c>
+      <c r="C108" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C109" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C107" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C109" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>